<commit_message>
estop aragones entries from agatha
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Wang_1996.xlsx
+++ b/ISRaD_data_files/Wang_1996.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="921">
   <si>
     <t>entry_name</t>
   </si>
@@ -538,9 +538,6 @@
   </si>
   <si>
     <t>control</t>
-  </si>
-  <si>
-    <t>19.4</t>
   </si>
   <si>
     <t>USDA</t>
@@ -3378,13 +3375,13 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G4" t="s">
         <v>48</v>
@@ -3578,13 +3575,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -3915,26 +3914,26 @@
       <c r="H4" t="s">
         <v>169</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="M4">
+        <v>127</v>
+      </c>
+      <c r="N4" t="s">
+        <v>915</v>
+      </c>
+      <c r="P4" t="s">
         <v>170</v>
       </c>
-      <c r="M4">
-        <v>12.7</v>
-      </c>
-      <c r="N4" t="s">
-        <v>916</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>171</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>172</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AA4" t="s">
         <v>173</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -3945,7 +3944,7 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H5" t="s">
         <v>169</v>
@@ -3954,19 +3953,19 @@
         <v>8.9</v>
       </c>
       <c r="M5">
-        <v>102</v>
+        <v>1020</v>
       </c>
       <c r="N5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="P5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T5" t="s">
+        <v>175</v>
+      </c>
+      <c r="U5" t="s">
         <v>176</v>
-      </c>
-      <c r="U5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -3977,7 +3976,7 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" t="s">
         <v>169</v>
@@ -3986,19 +3985,19 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="M6">
-        <v>86</v>
+        <v>860</v>
       </c>
       <c r="N6" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="P6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T6" t="s">
+        <v>178</v>
+      </c>
+      <c r="U6" t="s">
         <v>179</v>
-      </c>
-      <c r="U6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:36">
@@ -4009,7 +4008,7 @@
         <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H7" t="s">
         <v>169</v>
@@ -4018,19 +4017,19 @@
         <v>19.399999999999999</v>
       </c>
       <c r="M7">
-        <v>12.7</v>
+        <v>127</v>
       </c>
       <c r="N7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="P7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T7" t="s">
         <v>171</v>
       </c>
-      <c r="T7" t="s">
-        <v>172</v>
-      </c>
       <c r="U7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4066,103 +4065,103 @@
         <v>82</v>
       </c>
       <c r="E1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" t="s">
         <v>183</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>184</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>185</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>186</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>187</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>188</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>189</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>190</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>191</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>192</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>193</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>194</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>195</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>196</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>197</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>198</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>199</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>200</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>201</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>202</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>203</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>204</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>205</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>206</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>207</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>208</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>209</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>210</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>211</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>212</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>213</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>214</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -4176,103 +4175,103 @@
         <v>115</v>
       </c>
       <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
         <v>216</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>217</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>218</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>219</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>220</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>221</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>222</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>223</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>224</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>225</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>226</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>228</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>229</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>230</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>231</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>232</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>233</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>234</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>235</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>236</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>237</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>238</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>239</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>240</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>241</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>242</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>243</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>244</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>245</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>246</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>247</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -4295,25 +4294,25 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L3" t="s">
         <v>249</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>250</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>251</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>252</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>253</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>254</v>
-      </c>
-      <c r="R3" t="s">
-        <v>255</v>
       </c>
       <c r="S3" t="s">
         <v>149</v>
@@ -4322,7 +4321,7 @@
         <v>149</v>
       </c>
       <c r="U3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V3" t="s">
         <v>155</v>
@@ -4331,28 +4330,28 @@
         <v>155</v>
       </c>
       <c r="Z3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA3" t="s">
         <v>257</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC3" t="s">
         <v>258</v>
       </c>
-      <c r="AB3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>259</v>
       </c>
-      <c r="AE3" t="s">
-        <v>260</v>
-      </c>
       <c r="AF3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AG3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AH3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -4394,289 +4393,289 @@
         <v>82</v>
       </c>
       <c r="D1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" t="s">
         <v>261</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>262</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>263</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>264</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>265</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>266</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>267</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>268</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>269</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>270</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>271</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>272</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>273</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>274</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>275</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>276</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>277</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>278</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>279</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>280</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>281</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>282</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>283</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>284</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>285</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>286</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>287</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>288</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>289</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>290</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>291</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>292</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>293</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>294</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>295</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>296</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>297</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>298</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>299</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>300</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>301</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>302</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>303</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>304</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>305</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>306</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>307</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>308</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>309</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>310</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>311</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>312</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>313</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>314</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>315</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>316</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>317</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>318</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>319</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>320</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>321</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>322</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>323</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>324</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>325</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>326</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>327</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>328</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>329</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>330</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>331</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>332</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>333</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>334</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>335</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>336</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>337</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>338</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>339</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>340</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>341</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>342</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>343</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>344</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>345</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>346</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>347</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>348</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>349</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>350</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>351</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>352</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>353</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>354</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:98">
@@ -4690,289 +4689,289 @@
         <v>116</v>
       </c>
       <c r="D2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" t="s">
         <v>356</v>
       </c>
-      <c r="E2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>357</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>358</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>359</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>360</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>361</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>362</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>363</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>364</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>365</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>366</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>367</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>368</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>369</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>370</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>371</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>372</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>373</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>374</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>375</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>376</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>377</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>378</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>379</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>380</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>381</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>382</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>383</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>384</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>385</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>386</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>387</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>388</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>389</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>390</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>391</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>392</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>393</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>394</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>395</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>396</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>397</v>
       </c>
-      <c r="AW2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>398</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>399</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>400</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>401</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>402</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>403</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>404</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>405</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BI2" t="s">
         <v>406</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BJ2" t="s">
         <v>407</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>408</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>409</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>410</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>411</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>412</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BP2" t="s">
         <v>413</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
         <v>414</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>415</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
         <v>416</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BT2" t="s">
         <v>417</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>418</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
         <v>419</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
         <v>420</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
         <v>421</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BY2" t="s">
         <v>422</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
         <v>423</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CA2" t="s">
         <v>424</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>425</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
         <v>426</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CD2" t="s">
         <v>427</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>428</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CF2" t="s">
         <v>429</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CG2" t="s">
         <v>430</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
         <v>431</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>432</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CJ2" t="s">
         <v>433</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CK2" t="s">
         <v>434</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CL2" t="s">
         <v>435</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CM2" t="s">
         <v>436</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CN2" t="s">
         <v>437</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CO2" t="s">
         <v>438</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CP2" t="s">
         <v>439</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CQ2" t="s">
         <v>440</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CR2" t="s">
         <v>441</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CS2" t="s">
         <v>442</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CT2" t="s">
         <v>443</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:98">
@@ -5001,13 +5000,13 @@
         <v>149</v>
       </c>
       <c r="O3" t="s">
+        <v>444</v>
+      </c>
+      <c r="P3" t="s">
         <v>445</v>
       </c>
-      <c r="P3" t="s">
-        <v>446</v>
-      </c>
       <c r="Q3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S3" t="s">
         <v>155</v>
@@ -5025,34 +5024,34 @@
         <v>36</v>
       </c>
       <c r="X3" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC3" t="s">
         <v>447</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>448</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>449</v>
       </c>
-      <c r="AE3" t="s">
-        <v>450</v>
-      </c>
       <c r="AF3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AG3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AH3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AI3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AJ3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AK3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AL3" t="s">
         <v>155</v>
@@ -5076,142 +5075,142 @@
         <v>155</v>
       </c>
       <c r="AS3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AT3" t="s">
         <v>155</v>
       </c>
       <c r="AU3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AW3" t="s">
         <v>258</v>
       </c>
-      <c r="AV3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AW3" t="s">
+      <c r="AY3" t="s">
         <v>259</v>
       </c>
-      <c r="AY3" t="s">
-        <v>260</v>
-      </c>
       <c r="AZ3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BA3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BB3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BE3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BF3" t="s">
+        <v>451</v>
+      </c>
+      <c r="BG3" t="s">
         <v>452</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
+        <v>452</v>
+      </c>
+      <c r="BL3" t="s">
         <v>453</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BM3" t="s">
         <v>453</v>
       </c>
-      <c r="BL3" t="s">
+      <c r="BN3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>453</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>453</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>453</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>453</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>453</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>453</v>
+      </c>
+      <c r="CE3" t="s">
         <v>454</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="CF3" t="s">
         <v>454</v>
       </c>
-      <c r="BN3" t="s">
+      <c r="CG3" t="s">
         <v>454</v>
       </c>
-      <c r="BO3" t="s">
+      <c r="CH3" t="s">
         <v>454</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="CI3" t="s">
         <v>454</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="CJ3" t="s">
         <v>454</v>
       </c>
-      <c r="BS3" t="s">
+      <c r="CK3" t="s">
         <v>454</v>
       </c>
-      <c r="BT3" t="s">
+      <c r="CL3" t="s">
         <v>454</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="CM3" t="s">
         <v>454</v>
       </c>
-      <c r="BW3" t="s">
+      <c r="CN3" t="s">
         <v>454</v>
       </c>
-      <c r="BX3" t="s">
+      <c r="CO3" t="s">
         <v>454</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="CP3" t="s">
         <v>454</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CQ3" t="s">
         <v>454</v>
       </c>
-      <c r="CA3" t="s">
+      <c r="CR3" t="s">
         <v>454</v>
       </c>
-      <c r="CB3" t="s">
+      <c r="CS3" t="s">
         <v>454</v>
       </c>
-      <c r="CC3" t="s">
+      <c r="CT3" t="s">
         <v>454</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>454</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>455</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:98">
@@ -5222,19 +5221,19 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
+        <v>482</v>
+      </c>
+      <c r="E4" t="s">
+        <v>456</v>
+      </c>
+      <c r="I4" t="s">
+        <v>457</v>
+      </c>
+      <c r="J4" t="s">
         <v>483</v>
-      </c>
-      <c r="E4" t="s">
-        <v>457</v>
-      </c>
-      <c r="I4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J4" t="s">
-        <v>484</v>
       </c>
       <c r="BC4">
         <v>8.4000000000000005E-2</v>
@@ -5248,19 +5247,19 @@
         <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
+        <v>484</v>
+      </c>
+      <c r="E5" t="s">
+        <v>456</v>
+      </c>
+      <c r="I5" t="s">
+        <v>483</v>
+      </c>
+      <c r="J5" t="s">
         <v>485</v>
-      </c>
-      <c r="E5" t="s">
-        <v>457</v>
-      </c>
-      <c r="I5" t="s">
-        <v>484</v>
-      </c>
-      <c r="J5" t="s">
-        <v>486</v>
       </c>
       <c r="BC5">
         <v>7.2000000000000008E-2</v>
@@ -5274,19 +5273,19 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
+        <v>460</v>
+      </c>
+      <c r="E6" t="s">
         <v>461</v>
       </c>
-      <c r="E6" t="s">
-        <v>462</v>
-      </c>
       <c r="I6" t="s">
+        <v>457</v>
+      </c>
+      <c r="J6" t="s">
         <v>458</v>
-      </c>
-      <c r="J6" t="s">
-        <v>459</v>
       </c>
       <c r="BC6">
         <v>0.95200000000000007</v>
@@ -5300,19 +5299,19 @@
         <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="BC7">
         <v>0.8859999999999999</v>
@@ -5326,19 +5325,19 @@
         <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="BC8">
         <v>0.76</v>
@@ -5355,19 +5354,19 @@
         <v>168</v>
       </c>
       <c r="D9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E9" t="s">
         <v>456</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>457</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>458</v>
       </c>
-      <c r="J9" t="s">
+      <c r="AO9" t="s">
         <v>459</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:98">
@@ -5381,19 +5380,19 @@
         <v>168</v>
       </c>
       <c r="D10" t="s">
+        <v>462</v>
+      </c>
+      <c r="E10" t="s">
+        <v>456</v>
+      </c>
+      <c r="I10" t="s">
+        <v>458</v>
+      </c>
+      <c r="J10" t="s">
         <v>463</v>
       </c>
-      <c r="E10" t="s">
-        <v>457</v>
-      </c>
-      <c r="I10" t="s">
-        <v>459</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="AO10" t="s">
         <v>464</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:98">
@@ -5407,19 +5406,19 @@
         <v>168</v>
       </c>
       <c r="D11" t="s">
+        <v>471</v>
+      </c>
+      <c r="E11" t="s">
+        <v>456</v>
+      </c>
+      <c r="I11" t="s">
+        <v>463</v>
+      </c>
+      <c r="J11" t="s">
         <v>472</v>
       </c>
-      <c r="E11" t="s">
-        <v>457</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="AO11" t="s">
         <v>464</v>
-      </c>
-      <c r="J11" t="s">
-        <v>473</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:98">
@@ -5430,19 +5429,19 @@
         <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D12" t="s">
+        <v>466</v>
+      </c>
+      <c r="E12" t="s">
         <v>467</v>
       </c>
-      <c r="E12" t="s">
+      <c r="I12" t="s">
+        <v>457</v>
+      </c>
+      <c r="J12" t="s">
         <v>468</v>
-      </c>
-      <c r="I12" t="s">
-        <v>458</v>
-      </c>
-      <c r="J12" t="s">
-        <v>469</v>
       </c>
       <c r="BC12">
         <v>0.87400000000000011</v>
@@ -5456,19 +5455,19 @@
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
+        <v>469</v>
+      </c>
+      <c r="E13" t="s">
+        <v>467</v>
+      </c>
+      <c r="I13" t="s">
+        <v>468</v>
+      </c>
+      <c r="J13" t="s">
         <v>470</v>
-      </c>
-      <c r="E13" t="s">
-        <v>468</v>
-      </c>
-      <c r="I13" t="s">
-        <v>469</v>
-      </c>
-      <c r="J13" t="s">
-        <v>471</v>
       </c>
       <c r="BC13">
         <v>0.82</v>
@@ -5482,19 +5481,19 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
+        <v>474</v>
+      </c>
+      <c r="E14" t="s">
+        <v>467</v>
+      </c>
+      <c r="I14" t="s">
+        <v>470</v>
+      </c>
+      <c r="J14" t="s">
         <v>475</v>
-      </c>
-      <c r="E14" t="s">
-        <v>468</v>
-      </c>
-      <c r="I14" t="s">
-        <v>471</v>
-      </c>
-      <c r="J14" t="s">
-        <v>476</v>
       </c>
       <c r="BC14">
         <v>0.65200000000000002</v>
@@ -5508,19 +5507,19 @@
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
+        <v>476</v>
+      </c>
+      <c r="E15" t="s">
+        <v>467</v>
+      </c>
+      <c r="I15" t="s">
+        <v>475</v>
+      </c>
+      <c r="J15" t="s">
         <v>477</v>
-      </c>
-      <c r="E15" t="s">
-        <v>468</v>
-      </c>
-      <c r="I15" t="s">
-        <v>476</v>
-      </c>
-      <c r="J15" t="s">
-        <v>478</v>
       </c>
       <c r="BC15">
         <v>0.60699999999999998</v>
@@ -5534,19 +5533,19 @@
         <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" t="s">
+        <v>478</v>
+      </c>
+      <c r="E16" t="s">
+        <v>467</v>
+      </c>
+      <c r="I16" t="s">
+        <v>477</v>
+      </c>
+      <c r="J16" t="s">
         <v>479</v>
-      </c>
-      <c r="E16" t="s">
-        <v>468</v>
-      </c>
-      <c r="I16" t="s">
-        <v>478</v>
-      </c>
-      <c r="J16" t="s">
-        <v>480</v>
       </c>
       <c r="BC16">
         <v>0.51100000000000001</v>
@@ -5560,19 +5559,19 @@
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17" t="s">
+        <v>480</v>
+      </c>
+      <c r="E17" t="s">
+        <v>467</v>
+      </c>
+      <c r="I17" t="s">
+        <v>479</v>
+      </c>
+      <c r="J17" t="s">
         <v>481</v>
-      </c>
-      <c r="E17" t="s">
-        <v>468</v>
-      </c>
-      <c r="I17" t="s">
-        <v>480</v>
-      </c>
-      <c r="J17" t="s">
-        <v>482</v>
       </c>
       <c r="BC17">
         <v>0.45799999999999996</v>
@@ -5612,79 +5611,79 @@
         <v>82</v>
       </c>
       <c r="D1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E1" t="s">
         <v>487</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>488</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>489</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>490</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>491</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>492</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>493</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>494</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>495</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>496</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>497</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>498</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>499</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>500</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>501</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>502</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>503</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>504</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>505</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>506</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>507</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>508</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>509</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>510</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -5698,76 +5697,76 @@
         <v>116</v>
       </c>
       <c r="D2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" t="s">
         <v>219</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>220</v>
       </c>
-      <c r="F2" t="s">
-        <v>221</v>
-      </c>
       <c r="G2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H2" t="s">
         <v>512</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>513</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>514</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>515</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>516</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>517</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O2" t="s">
+        <v>233</v>
+      </c>
+      <c r="P2" t="s">
         <v>518</v>
       </c>
-      <c r="N2" t="s">
-        <v>233</v>
-      </c>
-      <c r="O2" t="s">
-        <v>234</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>519</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>520</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>239</v>
+      </c>
+      <c r="U2" t="s">
+        <v>240</v>
+      </c>
+      <c r="V2" t="s">
+        <v>241</v>
+      </c>
+      <c r="W2" t="s">
         <v>521</v>
       </c>
-      <c r="T2" t="s">
-        <v>240</v>
-      </c>
-      <c r="U2" t="s">
-        <v>241</v>
-      </c>
-      <c r="V2" t="s">
-        <v>242</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>522</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>523</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>524</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>525</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>526</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -5787,34 +5786,34 @@
         <v>158</v>
       </c>
       <c r="H3" t="s">
+        <v>527</v>
+      </c>
+      <c r="L3" t="s">
         <v>528</v>
       </c>
-      <c r="L3" t="s">
-        <v>529</v>
-      </c>
       <c r="M3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N3" t="s">
         <v>155</v>
       </c>
       <c r="R3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="X3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5832,7 +5831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
@@ -5849,214 +5848,214 @@
         <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E1" t="s">
+        <v>529</v>
+      </c>
+      <c r="F1" t="s">
         <v>530</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>531</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>532</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>533</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>534</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>535</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>536</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>537</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>538</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>539</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>540</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>542</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>543</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>544</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>545</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>546</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>547</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>548</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>549</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>550</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>551</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>552</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>553</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>554</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>555</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>556</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>557</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>558</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="AL1" t="s">
         <v>559</v>
       </c>
-      <c r="AI1" s="3" t="s">
-        <v>919</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>920</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>921</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>560</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>561</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>562</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>563</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>564</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>565</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>566</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>567</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>568</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>569</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>570</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>571</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>572</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>573</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>574</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>575</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>576</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>577</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>578</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>579</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>580</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>581</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>582</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>583</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>584</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>585</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>586</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>587</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>588</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>589</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>590</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>591</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>592</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>593</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>594</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:73">
@@ -6070,211 +6069,211 @@
         <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E2" t="s">
+        <v>595</v>
+      </c>
+      <c r="F2" t="s">
         <v>596</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>597</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>598</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>599</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>600</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>601</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>602</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>603</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>604</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>605</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>606</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>218</v>
+      </c>
+      <c r="R2" t="s">
+        <v>219</v>
+      </c>
+      <c r="S2" t="s">
+        <v>220</v>
+      </c>
+      <c r="U2" t="s">
         <v>607</v>
       </c>
-      <c r="Q2" t="s">
-        <v>219</v>
-      </c>
-      <c r="R2" t="s">
-        <v>220</v>
-      </c>
-      <c r="S2" t="s">
-        <v>221</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>608</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>609</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>610</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>611</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>612</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>613</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>614</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF2" t="s">
         <v>615</v>
       </c>
-      <c r="AC2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>616</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>617</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>618</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>619</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>620</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
+        <v>403</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>404</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>405</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>411</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>412</v>
+      </c>
+      <c r="AS2" t="s">
         <v>621</v>
       </c>
-      <c r="AL2" t="s">
-        <v>404</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>405</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>406</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>410</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>411</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>412</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>413</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>415</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>418</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>420</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>421</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>422</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>423</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>424</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>425</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>426</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>428</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>429</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>430</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>622</v>
       </c>
-      <c r="AT2" t="s">
-        <v>415</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>416</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>417</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>418</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>419</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>420</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>421</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>422</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>423</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>424</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>425</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>426</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>427</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>429</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>430</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>431</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>623</v>
-      </c>
       <c r="BK2" t="s">
+        <v>432</v>
+      </c>
+      <c r="BL2" t="s">
         <v>433</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>434</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>435</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>436</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BP2" t="s">
         <v>437</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
         <v>438</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>439</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
         <v>440</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BT2" t="s">
         <v>441</v>
       </c>
-      <c r="BT2" t="s">
-        <v>442</v>
-      </c>
       <c r="BU2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:73">
@@ -6282,19 +6281,19 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
+        <v>623</v>
+      </c>
+      <c r="G3" t="s">
         <v>624</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>625</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>626</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>627</v>
-      </c>
-      <c r="M3" t="s">
-        <v>628</v>
       </c>
       <c r="N3" t="s">
         <v>149</v>
@@ -6327,121 +6326,121 @@
         <v>155</v>
       </c>
       <c r="AA3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AB3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AE3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AF3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AG3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AH3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AL3" t="s">
+        <v>451</v>
+      </c>
+      <c r="AM3" t="s">
         <v>452</v>
       </c>
-      <c r="AM3" t="s">
-        <v>453</v>
-      </c>
       <c r="AN3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AO3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AP3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AQ3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AR3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AT3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AU3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AV3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AW3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AY3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AZ3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BA3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BB3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BD3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BE3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BF3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="BG3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BH3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BI3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BJ3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BK3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BL3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BM3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BN3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BO3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BP3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BQ3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BR3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BS3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BT3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="BU3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -6474,85 +6473,85 @@
         <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F1" t="s">
+        <v>629</v>
+      </c>
+      <c r="G1" t="s">
         <v>630</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>631</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>632</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>633</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>634</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>635</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>636</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>637</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>638</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>639</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>640</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>641</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>642</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>643</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>644</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>645</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>646</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>647</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>648</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>649</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>650</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>651</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>652</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>653</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -6563,79 +6562,79 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
+        <v>654</v>
+      </c>
+      <c r="D2" t="s">
         <v>655</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>656</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>657</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K2" t="s">
         <v>658</v>
       </c>
-      <c r="G2" t="s">
-        <v>362</v>
-      </c>
-      <c r="H2" t="s">
-        <v>219</v>
-      </c>
-      <c r="I2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J2" t="s">
-        <v>221</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>659</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>660</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>661</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>662</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>663</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>664</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>665</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
+        <v>239</v>
+      </c>
+      <c r="W2" t="s">
+        <v>240</v>
+      </c>
+      <c r="X2" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y2" t="s">
         <v>666</v>
       </c>
-      <c r="V2" t="s">
-        <v>240</v>
-      </c>
-      <c r="W2" t="s">
-        <v>241</v>
-      </c>
-      <c r="X2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>667</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>668</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>669</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>670</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>671</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -6652,37 +6651,37 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="M3" t="s">
         <v>151</v>
       </c>
       <c r="P3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="Q3" t="s">
         <v>155</v>
       </c>
       <c r="T3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="X3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AA3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -6706,136 +6705,136 @@
   <sheetData>
     <row r="1" spans="1:44">
       <c r="A1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B1" t="s">
         <v>675</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>676</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>677</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>678</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>679</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>680</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>681</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>682</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>683</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>684</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>685</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>686</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>687</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>688</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>689</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>690</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>691</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>692</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>693</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>694</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>695</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>696</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>697</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>698</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>699</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>700</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>701</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>702</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>703</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>704</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>705</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>706</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>707</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>708</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>709</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>710</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>711</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>712</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>713</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>714</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>715</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>716</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>717</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="2" spans="1:44">
@@ -6873,828 +6872,828 @@
         <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N2" t="s">
         <v>190</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>191</v>
       </c>
-      <c r="O2" t="s">
-        <v>192</v>
-      </c>
       <c r="P2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q2" t="s">
+        <v>195</v>
+      </c>
+      <c r="R2" t="s">
         <v>196</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>197</v>
       </c>
-      <c r="S2" t="s">
-        <v>198</v>
-      </c>
       <c r="T2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="W2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Y2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA2" t="s">
+        <v>718</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>490</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>492</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>493</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>629</v>
+      </c>
+      <c r="AH2" t="s">
         <v>719</v>
       </c>
-      <c r="AB2" t="s">
-        <v>491</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>492</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>493</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>494</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>500</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>630</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>720</v>
-      </c>
       <c r="AI2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AJ2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AK2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AL2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AM2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AP2" t="s">
         <v>533</v>
       </c>
-      <c r="AN2" t="s">
-        <v>537</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>534</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AR2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:44">
       <c r="G3" t="s">
+        <v>720</v>
+      </c>
+      <c r="H3" t="s">
         <v>721</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>722</v>
       </c>
-      <c r="I3" t="s">
+      <c r="U3" t="s">
+        <v>721</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>598</v>
+      </c>
+      <c r="AO3" t="s">
         <v>723</v>
       </c>
-      <c r="U3" t="s">
-        <v>722</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>599</v>
-      </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>724</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" t="s">
         <v>726</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>727</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>728</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" t="s">
         <v>729</v>
       </c>
-      <c r="E4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>730</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>731</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>732</v>
-      </c>
-      <c r="J4" t="s">
-        <v>733</v>
       </c>
       <c r="K4" t="s">
         <v>169</v>
       </c>
       <c r="L4" t="s">
+        <v>733</v>
+      </c>
+      <c r="M4" t="s">
         <v>734</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>735</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>736</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>737</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>738</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
+        <v>727</v>
+      </c>
+      <c r="S4" t="s">
+        <v>727</v>
+      </c>
+      <c r="T4" t="s">
         <v>739</v>
       </c>
-      <c r="R4" t="s">
-        <v>728</v>
-      </c>
-      <c r="S4" t="s">
-        <v>728</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>740</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>741</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>742</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>727</v>
+      </c>
+      <c r="Z4" t="s">
         <v>743</v>
       </c>
-      <c r="X4" t="s">
-        <v>728</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>728</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>744</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>745</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
+        <v>734</v>
+      </c>
+      <c r="AD4" t="s">
         <v>746</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
+        <v>737</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>747</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>748</v>
+      </c>
+      <c r="AH4" t="s">
         <v>735</v>
       </c>
-      <c r="AD4" t="s">
-        <v>747</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>738</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>748</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AI4" t="s">
         <v>749</v>
       </c>
-      <c r="AH4" t="s">
-        <v>736</v>
-      </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>750</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>751</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>752</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>753</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>754</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>755</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>756</v>
       </c>
-      <c r="AP4" t="s">
-        <v>757</v>
-      </c>
       <c r="AQ4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="AR4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="5" spans="1:44">
       <c r="A5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B5" t="s">
         <v>758</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>759</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>760</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>761</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>762</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>763</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>764</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>765</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>766</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>767</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>768</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>769</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>770</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>771</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>772</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>773</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>774</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>775</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>776</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AA5" t="s">
         <v>777</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>778</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
+        <v>768</v>
+      </c>
+      <c r="AD5" t="s">
         <v>779</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AE5" t="s">
+        <v>771</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>780</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>781</v>
+      </c>
+      <c r="AH5" t="s">
         <v>769</v>
       </c>
-      <c r="AD5" t="s">
-        <v>780</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>772</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>781</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AI5" t="s">
         <v>782</v>
       </c>
-      <c r="AH5" t="s">
-        <v>770</v>
-      </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>783</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>784</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>785</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>786</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>787</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>788</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>789</v>
       </c>
-      <c r="AP5" t="s">
-        <v>790</v>
-      </c>
       <c r="AR5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="6" spans="1:44">
       <c r="A6" t="s">
+        <v>790</v>
+      </c>
+      <c r="B6" t="s">
         <v>791</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>792</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>793</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
         <v>794</v>
       </c>
-      <c r="F6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>795</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>796</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>797</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>798</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>799</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>800</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>801</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>802</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
+        <v>528</v>
+      </c>
+      <c r="T6" t="s">
         <v>803</v>
       </c>
-      <c r="Q6" t="s">
-        <v>529</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>804</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>805</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>806</v>
       </c>
-      <c r="W6" t="s">
+      <c r="AA6" t="s">
         <v>807</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>808</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
+        <v>799</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>802</v>
+      </c>
+      <c r="AF6" t="s">
         <v>809</v>
       </c>
-      <c r="AC6" t="s">
-        <v>800</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>803</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>810</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>811</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>812</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
+        <v>793</v>
+      </c>
+      <c r="AM6" t="s">
         <v>813</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>794</v>
-      </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>814</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>815</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>816</v>
       </c>
       <c r="AP6" t="s">
         <v>36</v>
       </c>
       <c r="AR6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="7" spans="1:44">
       <c r="A7" t="s">
+        <v>816</v>
+      </c>
+      <c r="B7" t="s">
         <v>817</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" t="s">
         <v>818</v>
       </c>
-      <c r="F7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>819</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>820</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>821</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>822</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>823</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>824</v>
       </c>
-      <c r="P7" t="s">
+      <c r="T7" t="s">
         <v>825</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>826</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>827</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>828</v>
       </c>
-      <c r="W7" t="s">
+      <c r="AC7" t="s">
+        <v>822</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF7" t="s">
         <v>829</v>
       </c>
-      <c r="AC7" t="s">
-        <v>823</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>825</v>
-      </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>830</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AI7" t="s">
         <v>831</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AM7" t="s">
         <v>832</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>833</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>834</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>835</v>
       </c>
-      <c r="AP7" t="s">
-        <v>836</v>
-      </c>
       <c r="AR7" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="8" spans="1:44">
       <c r="A8" t="s">
+        <v>836</v>
+      </c>
+      <c r="B8" t="s">
         <v>837</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>838</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>839</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>840</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>841</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>842</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>843</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>844</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>845</v>
       </c>
-      <c r="P8" t="s">
+      <c r="T8" t="s">
         <v>846</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>847</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>848</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
+        <v>793</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>843</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>845</v>
+      </c>
+      <c r="AG8" t="s">
         <v>849</v>
       </c>
-      <c r="W8" t="s">
-        <v>794</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>844</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>846</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AM8" t="s">
         <v>850</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AN8" t="s">
         <v>851</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
         <v>852</v>
       </c>
-      <c r="AO8" t="s">
-        <v>853</v>
-      </c>
       <c r="AP8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AR8" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="9" spans="1:44">
       <c r="A9" t="s">
+        <v>853</v>
+      </c>
+      <c r="B9" t="s">
         <v>854</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F9" t="s">
         <v>855</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>856</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>857</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>858</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>859</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>860</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
         <v>861</v>
       </c>
-      <c r="P9" t="s">
+      <c r="T9" t="s">
         <v>862</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>863</v>
       </c>
-      <c r="U9" t="s">
+      <c r="AE9" t="s">
         <v>864</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AG9" t="s">
+        <v>860</v>
+      </c>
+      <c r="AM9" t="s">
         <v>865</v>
       </c>
-      <c r="AG9" t="s">
-        <v>861</v>
-      </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>866</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>867</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>868</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="10" spans="1:44">
       <c r="A10" t="s">
+        <v>869</v>
+      </c>
+      <c r="B10" t="s">
         <v>870</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>871</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>872</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>873</v>
       </c>
-      <c r="H10" t="s">
+      <c r="U10" t="s">
         <v>874</v>
       </c>
-      <c r="U10" t="s">
+      <c r="AM10" t="s">
         <v>875</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>876</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>877</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>878</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="11" spans="1:44">
       <c r="B11" t="s">
+        <v>879</v>
+      </c>
+      <c r="F11" t="s">
         <v>880</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>881</v>
       </c>
-      <c r="H11" t="s">
+      <c r="U11" t="s">
         <v>882</v>
       </c>
-      <c r="U11" t="s">
+      <c r="AM11" t="s">
         <v>883</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AN11" t="s">
         <v>884</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AO11" t="s">
+        <v>884</v>
+      </c>
+      <c r="AP11" t="s">
         <v>885</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>885</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="12" spans="1:44">
       <c r="H12" t="s">
+        <v>886</v>
+      </c>
+      <c r="U12" t="s">
         <v>887</v>
       </c>
-      <c r="U12" t="s">
+      <c r="AM12" t="s">
         <v>888</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>889</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>890</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="13" spans="1:44">
       <c r="U13" t="s">
+        <v>891</v>
+      </c>
+      <c r="AM13" t="s">
         <v>892</v>
       </c>
-      <c r="AM13" t="s">
+      <c r="AN13" t="s">
         <v>893</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>894</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="14" spans="1:44">
       <c r="U14" t="s">
+        <v>895</v>
+      </c>
+      <c r="AN14" t="s">
         <v>896</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>897</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="15" spans="1:44">
       <c r="U15" t="s">
+        <v>898</v>
+      </c>
+      <c r="AN15" t="s">
         <v>899</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>900</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="16" spans="1:44">
       <c r="U16" t="s">
+        <v>901</v>
+      </c>
+      <c r="AN16" t="s">
         <v>902</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AO16" t="s">
         <v>903</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="17" spans="40:41">
       <c r="AN17" t="s">
+        <v>904</v>
+      </c>
+      <c r="AO17" t="s">
         <v>905</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="18" spans="40:41">
       <c r="AN18" t="s">
+        <v>906</v>
+      </c>
+      <c r="AO18" t="s">
         <v>907</v>
-      </c>
-      <c r="AO18" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="19" spans="40:41">
       <c r="AN19" t="s">
+        <v>908</v>
+      </c>
+      <c r="AO19" t="s">
         <v>909</v>
-      </c>
-      <c r="AO19" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="20" spans="40:41">
       <c r="AN20" t="s">
+        <v>910</v>
+      </c>
+      <c r="AO20" t="s">
         <v>911</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="21" spans="40:41">
       <c r="AN21" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>